<commit_message>
modify figures based on Nat Commn reviewers suggestions
</commit_message>
<xml_diff>
--- a/results/outputs/res_ancombc2.xlsx
+++ b/results/outputs/res_ancombc2.xlsx
@@ -7,15 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="group_species" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="group_genus" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="status_species" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="status_genus" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="status_species" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">taxon</t>
   </si>
@@ -113,54 +111,6 @@
     <t xml:space="preserve">Succinivibrio spp.</t>
   </si>
   <si>
-    <t xml:space="preserve">Akkermansia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alistipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anaerovibrio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacteroides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bifidobacterium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Butyricimonas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dehalobacterium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lachnobacterium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lachnospira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lactococcus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Megasphaera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methanobrevibacter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odoribacter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paraprevotella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFN20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Succinivibrio</t>
-  </si>
-  <si>
     <t xml:space="preserve">lfc_(Intercept)</t>
   </si>
   <si>
@@ -285,42 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">V.dispar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Eubacterium]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anaerostipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anaerotruncus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilophila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christensenella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clostridium_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clostridium_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holdemania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lactobacillus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methanosphaera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phascolarctobacterium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMB53</t>
   </si>
 </sst>
 </file>
@@ -1469,727 +1383,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.000000000855671996230367</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-0.397961751738174</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-1.27757619244244</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.363983112451788</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.327996128846641</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.398068925999307</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1.27757619244244</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.105293433726283</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.144900061006886</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.713031812880188</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.992174258334821</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.365011847246202</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.321983479342453</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.394898626391692</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.992174258334821</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="n">
-        <v>-0.916556451257714</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.916556451200002</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.916556451576919</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.310866068097343</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.277872018749636</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.362765135108711</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.916556451576919</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.505408481886161</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-0.403080296001189</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.673425938257623</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-1.42523230539252</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.347584447765032</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.310787842559312</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.419500656106693</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.42523230539252</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.00000000000159847405030625</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-0.000000000178913480757675</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.963382882530012</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.361432716593131</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.322076906622269</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.407348824061057</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.963382882530012</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-0.000000000189990488736016</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.272097486929234</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.754970823361427</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.299815653170371</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.268488230635584</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.334332404998898</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.754970823361427</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.576343005659657</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.451705572941777</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.670597914778859</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.833041796357211</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.299908139657036</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.266566079881905</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.345028331543917</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.833041796357211</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.186614199665659</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.186614199729873</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.768885579403154</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.30444025677256</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.273551240024017</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.353467988865773</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.768885579403154</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.576343005659657</v>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.211863036361099</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-0.21186303641292</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.89449740765151</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.275516751821162</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.257353422791364</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.331395040646732</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.89449740765151</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.623844330460877</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.847460538930665</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.24385152142815</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.31013359318354</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.277369608435614</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.371561631291975</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.24385152142815</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="n">
-        <v>-0.243859021410361</v>
-      </c>
-      <c r="C12" t="n">
-        <v>-0.243859021609156</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-1.09825654928012</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.313823590766147</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.275727834982806</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.417672591369215</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1.09825654928012</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="n">
-        <v>0.959642507061196</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.959642507959523</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.959642508063098</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.357503478543766</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.297993817805026</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.39567032395604</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.959642508063098</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="n">
-        <v>-0.154967774382656</v>
-      </c>
-      <c r="C14" t="n">
-        <v>-0.352949517916632</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-0.814380188950442</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.279576199165308</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.256966022319037</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.339893592071227</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.814380188950442</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.511425249527663</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="n">
-        <v>-0.0000000000709914807922655</v>
-      </c>
-      <c r="C15" t="n">
-        <v>-0.000000000167273742203669</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-0.84378360299259</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.322816220897534</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.28678280160239</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.359440539254624</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.84378360299259</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.022</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.545048362818409</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="n">
-        <v>0.615009718967571</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.615009718968573</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.890133857743342</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.308487180471913</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.28539813068011</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.397759529156529</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.890133857743342</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.034</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.68190033270355</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="n">
-        <v>-1.03573658980877</v>
-      </c>
-      <c r="C17" t="n">
-        <v>-1.03573659005626</v>
-      </c>
-      <c r="D17" t="n">
-        <v>-1.03573659127603</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.361261072065581</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.32777320181238</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.451717569547554</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1.03573659127603</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.545048362818409</v>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="V1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" t="s">
-        <v>67</v>
-      </c>
-      <c r="V1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2">
@@ -2262,7 +1516,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B3" t="n">
         <v>-0.419697831661367</v>
@@ -2330,7 +1584,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B4" t="n">
         <v>0.0297030649716383</v>
@@ -2398,7 +1652,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B5" t="n">
         <v>-0.508887942757413</v>
@@ -2534,7 +1788,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B7" t="n">
         <v>-0.542493718360467</v>
@@ -2670,7 +1924,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B9" t="n">
         <v>-0.0690091591297553</v>
@@ -2874,7 +2128,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B12" t="n">
         <v>-0.253253744875526</v>
@@ -3010,7 +2264,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B14" t="n">
         <v>0.204216532540425</v>
@@ -3078,7 +2332,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B15" t="n">
         <v>-0.486651757438504</v>
@@ -3146,7 +2400,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B16" t="n">
         <v>-0.544556270390957</v>
@@ -3214,7 +2468,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B17" t="n">
         <v>-0.762632584454213</v>
@@ -3350,7 +2604,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
         <v>-0.0948046002614429</v>
@@ -3418,7 +2672,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B20" t="n">
         <v>-0.0995888733926204</v>
@@ -3486,7 +2740,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B21" t="n">
         <v>-0.297584986772255</v>
@@ -3554,7 +2808,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B22" t="n">
         <v>-0.30077638027966</v>
@@ -3622,7 +2876,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B23" t="n">
         <v>-0.413135859228529</v>
@@ -3758,7 +3012,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B25" t="n">
         <v>0.0145722333278142</v>
@@ -3894,7 +3148,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B27" t="n">
         <v>-0.230177556615076</v>
@@ -3962,7 +3216,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B28" t="n">
         <v>0.176506443634315</v>
@@ -4030,7 +3284,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B29" t="n">
         <v>-0.298515542604418</v>
@@ -4098,7 +3352,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B30" t="n">
         <v>-0.29847583179127</v>
@@ -4166,7 +3420,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B31" t="n">
         <v>-0.192625976594126</v>
@@ -4229,1380 +3483,6 @@
         <v>1</v>
       </c>
       <c r="V31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" t="s">
-        <v>67</v>
-      </c>
-      <c r="V1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.126663270232511</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.681540483196164</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.30271902168841</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.140533423030488</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.192458095897465</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.200312043668501</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-0.901303529801815</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3.54124091282325</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-1.51123724836727</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.368426197061945</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.000487341312529386</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.132182864038548</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.0244407026153022</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.413730309242648</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.371861992331899</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.935460985753178</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.142700227817873</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.182601349252625</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.178563630753874</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-2.89929676756149</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-2.03646902859099</v>
-      </c>
-      <c r="J3" t="n">
-        <v>5.238810287424</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.00514206915787602</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.0459116350356422</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.00000198789585077496</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.165780270997955</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.790167092441565</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.000224314115502208</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" t="b">
-        <v>0</v>
-      </c>
-      <c r="U3" t="b">
-        <v>0</v>
-      </c>
-      <c r="V3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0382440516535556</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.624284713493624</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.062670700886062</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.150208489034387</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.221593102546342</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.214636762713869</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.254606459990423</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-2.81725697379532</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.291984933492535</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.799349979420445</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.0054465864179303</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.770671724092665</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.155516705945646</v>
-      </c>
-      <c r="P4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="b">
-        <v>0</v>
-      </c>
-      <c r="V4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.0297030649716383</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.394497668708514</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.245466870277015</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0717712913294406</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.124445281943876</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.113141719617946</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.413857190269811</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-3.17004921798828</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-2.16955223153671</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.6800089981047</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.00211199171709973</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.0327994998655802</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.0794390299311584</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.643668643811337</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-0.508887942757413</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.311099732445288</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.157091430465152</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0567427373849914</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.101575968128734</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0854450423269927</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-8.96833614678616</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3.06272968081396</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.83850842818912</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.00000000572151236000963</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.00551282319052271</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.0789367652797156</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.00000086082040556949</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.155516705945646</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.124709249612661</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.82522663555975</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.353306298084922</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.165588415088422</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.231778677704564</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.219429252326982</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.753127865533758</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-3.56040790176404</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.61011485177211</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.452153444653929</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.000450976215411214</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.10876246704385</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.0244407026153022</v>
-      </c>
-      <c r="P7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="b">
-        <v>1</v>
-      </c>
-      <c r="U7" t="b">
-        <v>1</v>
-      </c>
-      <c r="V7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-0.253253744875526</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-0.499071102015205</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.571568763100673</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0986261771814889</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.149817564345363</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.139117426570872</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-2.56781467266541</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-3.33119220163487</v>
-      </c>
-      <c r="J8" t="n">
-        <v>4.10853461848285</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0116276998176677</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.0011909427290421</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.0000786370484073827</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.291570964780955</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.0537543784851143</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.00507051569910818</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U8" t="b">
-        <v>1</v>
-      </c>
-      <c r="V8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.250152007819805</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.487609461551033</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.184084850747015</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.10649600633192</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.152901533433303</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.146632890297194</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.34893322703715</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-3.18904232418136</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-1.25541309575167</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.020072745075452</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.00172343073815541</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.211194123498638</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.467705398801021</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.0707170469643592</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="b">
-        <v>1</v>
-      </c>
-      <c r="U9" t="b">
-        <v>1</v>
-      </c>
-      <c r="V9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.762632584454213</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.379268034772493</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.549394037974777</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.0543371928571632</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.111404382571014</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.0926456498446337</v>
-      </c>
-      <c r="H10" t="n">
-        <v>-14.035185558057</v>
-      </c>
-      <c r="I10" t="n">
-        <v>3.40442652272437</v>
-      </c>
-      <c r="J10" t="n">
-        <v>5.93005757848435</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.00000000000185714510847289</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.00254428925555911</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.00000573796002192256</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.000000000838240820722969</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.0883377023569183</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.000517977006331723</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="b">
-        <v>0</v>
-      </c>
-      <c r="U10" t="b">
-        <v>1</v>
-      </c>
-      <c r="V10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.43565050731072</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.336055968714107</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0286824178578934</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0798388277267319</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.126243188621939</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.117619483154471</v>
-      </c>
-      <c r="H11" t="n">
-        <v>-5.45662454867</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2.66197307262647</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.243857710378003</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.000000811392173423282</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.00977899828196747</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.808109071054724</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.0000610383143348627</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.243669575872903</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" t="b">
-        <v>0</v>
-      </c>
-      <c r="U11" t="b">
-        <v>1</v>
-      </c>
-      <c r="V11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" t="n">
-        <v>-0.454769710291132</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.250203173446643</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-0.0970498022798277</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0684811027496536</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.123288940737695</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.10802054960345</v>
-      </c>
-      <c r="H12" t="n">
-        <v>-6.64080588704352</v>
-      </c>
-      <c r="I12" t="n">
-        <v>2.0294048432046</v>
-      </c>
-      <c r="J12" t="n">
-        <v>-0.898438330818566</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.0000000146037972227383</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.0472671846643521</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.372868370721982</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.00000131831367552383</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.790167092441565</v>
-      </c>
-      <c r="P12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="n">
-        <v>-0.191493187638733</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.481786679304266</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.246461204371487</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.0734097079996805</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.110951631873727</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.0980506071929308</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-2.60855400268812</v>
-      </c>
-      <c r="I13" t="n">
-        <v>4.34231269218808</v>
-      </c>
-      <c r="J13" t="n">
-        <v>-2.5136122195198</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.0115452871655627</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.0000573146717466601</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.0147491287580078</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.291570964780955</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.0036956491725774</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.332858260204219</v>
-      </c>
-      <c r="Q13" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
-        <v>1</v>
-      </c>
-      <c r="S13" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" t="b">
-        <v>0</v>
-      </c>
-      <c r="V13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" t="n">
-        <v>-0.413135859228529</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.221310098053433</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.0907000982129725</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0631151699883655</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.10895888185423</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.0953420838117518</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-6.54574580571811</v>
-      </c>
-      <c r="I14" t="n">
-        <v>2.03113407817008</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.951312312326373</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.0000000103194616013398</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.0462723034426887</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.344916740839991</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.00000116444777560209</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.790167092441565</v>
-      </c>
-      <c r="P14" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" t="b">
-        <v>0</v>
-      </c>
-      <c r="U14" t="b">
-        <v>1</v>
-      </c>
-      <c r="V14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.0760136677504597</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.666273946623447</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-1.05109905210904</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0655402012063562</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.117103093407087</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.101878473236637</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1.15980217257996</v>
-      </c>
-      <c r="I15" t="n">
-        <v>5.68963574947821</v>
-      </c>
-      <c r="J15" t="n">
-        <v>-10.3171849627901</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.256283108732335</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.00000481124116420482</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.0000000000723539299246709</v>
-      </c>
-      <c r="N15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.000434320261112547</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.0000000163288310983034</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" t="b">
-        <v>1</v>
-      </c>
-      <c r="S15" t="b">
-        <v>1</v>
-      </c>
-      <c r="T15" t="b">
-        <v>1</v>
-      </c>
-      <c r="U15" t="b">
-        <v>1</v>
-      </c>
-      <c r="V15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="n">
-        <v>-0.223278324455721</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.54738684341942</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.0891322938179787</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.13309861443404</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.197884371147796</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.181339038744956</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-1.67754056197461</v>
-      </c>
-      <c r="I16" t="n">
-        <v>2.76619543142489</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.491522919912125</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.096689898282572</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.0068032981311794</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.62417858596618</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.180631525208325</v>
-      </c>
-      <c r="P16" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" t="b">
-        <v>1</v>
-      </c>
-      <c r="U16" t="b">
-        <v>0</v>
-      </c>
-      <c r="V16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.0145722333278142</v>
-      </c>
-      <c r="C17" t="n">
-        <v>-0.686517377524989</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.447261718186881</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0713305029474202</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.11595508988546</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.0988041288032307</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.204291750733285</v>
-      </c>
-      <c r="I17" t="n">
-        <v>-5.92054543015859</v>
-      </c>
-      <c r="J17" t="n">
-        <v>4.52675129677634</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.83977952450422</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.00000352588200748647</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.000127066050386638</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.000397860432962898</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.00592288878074988</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
-        <v>1</v>
-      </c>
-      <c r="S17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T17" t="b">
-        <v>1</v>
-      </c>
-      <c r="U17" t="b">
-        <v>0</v>
-      </c>
-      <c r="V17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.0747552566451606</v>
-      </c>
-      <c r="C18" t="n">
-        <v>-0.381211566866364</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-0.0230717024127228</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0925254314509555</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.154932410740386</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.139258617622052</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.807942805268471</v>
-      </c>
-      <c r="I18" t="n">
-        <v>-2.46050238968491</v>
-      </c>
-      <c r="J18" t="n">
-        <v>-0.165675222163553</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.420446998256318</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.0150487560681822</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.868643319009681</v>
-      </c>
-      <c r="N18" t="n">
-        <v>1</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.323447855013015</v>
-      </c>
-      <c r="P18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="b">
-        <v>0</v>
-      </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S18" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" t="b">
-        <v>0</v>
-      </c>
-      <c r="U18" t="b">
-        <v>1</v>
-      </c>
-      <c r="V18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" t="n">
-        <v>-0.230177556615076</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.479536314108903</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.124063563679348</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.135368598609163</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.201114598514251</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.192662823556636</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-1.70037629834409</v>
-      </c>
-      <c r="I19" t="n">
-        <v>2.38439336403977</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.643941375866312</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.0905916181976024</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.0180281420962448</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0.520340320156962</v>
-      </c>
-      <c r="N19" t="n">
-        <v>1</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0.36987183269831</v>
-      </c>
-      <c r="P19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="b">
-        <v>0</v>
-      </c>
-      <c r="R19" t="b">
-        <v>0</v>
-      </c>
-      <c r="S19" t="b">
-        <v>0</v>
-      </c>
-      <c r="T19" t="b">
-        <v>1</v>
-      </c>
-      <c r="U19" t="b">
-        <v>0</v>
-      </c>
-      <c r="V19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.29847583179127</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.273297579710426</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.105611177182516</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.0786167806325452</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.12388433895707</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.109736060881986</v>
-      </c>
-      <c r="H20" t="n">
-        <v>-3.79659189030324</v>
-      </c>
-      <c r="I20" t="n">
-        <v>2.20607045257861</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.962410864156077</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.000362825541829668</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.0314984921583826</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.339980720075487</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.014887718034378</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0.592381504410503</v>
-      </c>
-      <c r="P20" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="b">
-        <v>1</v>
-      </c>
-      <c r="R20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S20" t="b">
-        <v>0</v>
-      </c>
-      <c r="T20" t="b">
-        <v>0</v>
-      </c>
-      <c r="U20" t="b">
-        <v>1</v>
-      </c>
-      <c r="V20" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>